<commit_message>
invalid data to test
</commit_message>
<xml_diff>
--- a/TechTests/JohnU_Lorien/WebApplication2/WebApplication2/Content/test.xlsx
+++ b/TechTests/JohnU_Lorien/WebApplication2/WebApplication2/Content/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file1\folderredir$\Desktops\GayatriP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\G A Y A T R I\code\GIT\TechTests\JohnU_Lorien\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Account</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>AUD</t>
+  </si>
+  <si>
+    <t>A1004</t>
+  </si>
+  <si>
+    <t>A1005</t>
+  </si>
+  <si>
+    <t>A1006</t>
+  </si>
+  <si>
+    <t>A1007</t>
   </si>
 </sst>
 </file>
@@ -388,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -431,14 +443,8 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3">
-        <v>10000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -466,6 +472,53 @@
         <v>15</v>
       </c>
       <c r="D5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
         <v>10000</v>
       </c>
     </row>

</xml_diff>